<commit_message>
removed columns from excel_file_metadata & changed main executor
</commit_message>
<xml_diff>
--- a/excel_files/filelist_metadata.xlsx
+++ b/excel_files/filelist_metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>file_name</t>
   </si>
@@ -62,24 +62,6 @@
   </si>
   <si>
     <t>order_status</t>
-  </si>
-  <si>
-    <t>file_separator</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>;</t>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>file_extension</t>
-  </si>
-  <si>
-    <t>csv</t>
   </si>
   <si>
     <t>file1_target</t>
@@ -418,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,7 +413,7 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,14 +423,8 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -458,14 +434,8 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -475,14 +445,8 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -492,14 +456,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -508,12 +466,6 @@
       </c>
       <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -523,10 +475,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,7 +488,7 @@
     <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,79 +498,49 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -645,10 +567,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>